<commit_message>
Resolve "Replace remaining old icons using svgs"
</commit_message>
<xml_diff>
--- a/src/resources/icons/icons.xlsx
+++ b/src/resources/icons/icons.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20395"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\devel\c++\GTlab-Core-2-0\src\resources\icons\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\devel\c++\GTlab-Core-2-0 (2)\src\resources\icons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001DFAE1-B356-4CA5-8255-36E338968455}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2861106F-3E29-420E-B925-5997BD2B5A44}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15420" xr2:uid="{BC4D2855-96DD-4C88-BDD9-0E8565547965}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -54,7 +54,10 @@
     <t>SVGs sind, wenn nicht anders angegeben, von:</t>
   </si>
   <si>
-    <t>Dateien mit Endung "_custom" wurden auf Basis anderer Dateien erstellt</t>
+    <t>Dateien mit Endung "_custom" wurden auf Basis anderer Dateien oder eigenständig erstellt</t>
+  </si>
+  <si>
+    <t>Alle svg Icons im ordner "letters" wurden eigenständig erstellt</t>
   </si>
 </sst>
 </file>
@@ -475,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{413131F0-930A-4E5F-940B-C714E9A34C92}">
-  <dimension ref="A2:E6"/>
+  <dimension ref="A2:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,22 +516,27 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>